<commit_message>
Add various options to control SNR and a playful noise monitor
</commit_message>
<xml_diff>
--- a/data-raw/SAA.xlsx
+++ b/data-raw/SAA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mary/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/SAA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9253840-685F-7A45-BA44-A1142E6A93EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3421FD82-F893-9641-99F8-0B21A984D8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - SAA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>key</t>
   </si>
@@ -230,13 +230,49 @@
   </si>
   <si>
     <t>Inserisci un nome utente per vedere il punteggio:</t>
+  </si>
+  <si>
+    <t>sing_favourite_song_page_title</t>
+  </si>
+  <si>
+    <t>Sing your favourite song!</t>
+  </si>
+  <si>
+    <t>When you are ready, click "Record" and sing your favourite song.</t>
+  </si>
+  <si>
+    <t>Sing the song!</t>
+  </si>
+  <si>
+    <t>When you are ready, click "Record" and sing back the song you hear.</t>
+  </si>
+  <si>
+    <t>Sing Happy Birthday</t>
+  </si>
+  <si>
+    <t>When you are ready, click "Record" and sing back Happy Birthday after you hear it.</t>
+  </si>
+  <si>
+    <t>sing_favourite_song_page_text</t>
+  </si>
+  <si>
+    <t>sing_the_song_page_title</t>
+  </si>
+  <si>
+    <t>sing_the_song_page_text</t>
+  </si>
+  <si>
+    <t>sing_hbd_page_text</t>
+  </si>
+  <si>
+    <t>sing_hbd_page_title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -247,6 +283,19 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -275,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -417,13 +466,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -478,18 +555,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1619,8 +1708,8 @@
   </sheetPr>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1785,7 +1874,7 @@
       <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
     </row>
@@ -1799,7 +1888,7 @@
       <c r="C11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
     </row>
@@ -1813,7 +1902,7 @@
       <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
     </row>
@@ -1827,7 +1916,7 @@
       <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
@@ -1841,7 +1930,7 @@
       <c r="C14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
     </row>
@@ -1919,71 +2008,119 @@
       <c r="C19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="20" t="s">
         <v>60</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="A21" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>71</v>
+      </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="A22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="A23" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="A24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>74</v>
+      </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+      <c r="A25" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>75</v>
+      </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="A26" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>76</v>
+      </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>

</xml_diff>

<commit_message>
Update Latvian and German translations
</commit_message>
<xml_diff>
--- a/data-raw/SAA.xlsx
+++ b/data-raw/SAA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/SAA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3421FD82-F893-9641-99F8-0B21A984D8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CD4134-A3DC-EF4C-84D0-42061CD69532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="2380" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - SAA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
   <si>
     <t>key</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Ti verrà chiesto di imitare alcuni suoni. Per favore, canta queste note sulla sillaba "daah", come nella prima parte della parola "dado" [rima con "fa la la"].</t>
   </si>
   <si>
-    <t>Sie werden gebeten werden einige Töne nachzuahmen. Bitte singen Sie diese Noten auf der Sylbe "daah" nach, so wie am Anfang des Names "David".</t>
-  </si>
-  <si>
     <t>SAA_instructions3</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>Cerca di produrre note che siano più stabili possibile, senza vibrato.  Ovvero, cerca di non far traballare la voce. Il computer può analizzare meglio un suono "fermo".</t>
   </si>
   <si>
-    <t>Versuchen Sie Töne zu produzieren, die so stabil wie möglich sind, ohne Vibrato. Das bedeutet, versuchen Sie Ihre Töne nicht flattern zu lassen. Der Computer can einen "klaren" Ton besser analysieren.</t>
-  </si>
-  <si>
     <t>SAA_instructions4</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>Dopo aver ascoltato la melodia, fai del tuo meglio per cantarla, poi clicca su Stop. Puoi provare ogni melodia fino a 3 volte. Va bene anche se pensi di non aver capito, semplicemente fai del tuo meglio!</t>
   </si>
   <si>
-    <t>Nachdem Sie die Melodie gehört haben, versuchen Sie diese bestmöglich nachzusingen. Dann klicken Sie auf Stop. Sie können jede Melodie bis zu dreimal versuchen. Es ist okay wenn Sie denken, dass Sie das nicht ganz geschafft haben. Versuchen Sie einfach Ihr Bestes!</t>
-  </si>
-  <si>
     <t>task_name</t>
   </si>
   <si>
@@ -266,13 +257,139 @@
   </si>
   <si>
     <t>sing_hbd_page_title</t>
+  </si>
+  <si>
+    <t>Sie werden gleich gebeten, einige Töne nachzuahmen. Bitte singen Sie diese Noten auf der Silbe "daah" nach, so wie am Anfang des Names "David".</t>
+  </si>
+  <si>
+    <t>Versuchen Sie Töne zu produzieren, die so stabil wie möglich sind, ohne Vibrato. Das bedeutet, versuchen Sie Ihre Töne nicht flattern zu lassen. Der Computer kann einen "klaren" Ton besser analysieren.</t>
+  </si>
+  <si>
+    <t>Sie haben bis zu</t>
+  </si>
+  <si>
+    <t>Sie haben</t>
+  </si>
+  <si>
+    <t>Versuche, um die Melodie so gut wie Sie können, nachzumachen</t>
+  </si>
+  <si>
+    <t>Versuch, um die Melodie so gut wie Sie können, nachzumachen.</t>
+  </si>
+  <si>
+    <t>Nutzen Sie so viele Versuche, wie Sie benötigen. Es ist spannend für uns, Verbesserungen zu sehen.</t>
+  </si>
+  <si>
+    <t>Nachdem Sie die Melodie gehört haben, versuchen Sie diese bestmöglichst nachzusingen. Dann klicken Sie auf Stop. Sie können jede Melodie bis zu dreimal versuchen. Es ist okay wenn Sie denken, dass Sie das nicht ganz geschafft haben. Versuchen Sie einfach Ihr Bestes!</t>
+  </si>
+  <si>
+    <t>Test zur Gesangsfähigkeit</t>
+  </si>
+  <si>
+    <t>Geben Sie einen Nutzernamen ein, um die Punktetafel zu sehen</t>
+  </si>
+  <si>
+    <t>Singen Sie Ihr Lieblingslied!</t>
+  </si>
+  <si>
+    <t>Wenn Sie bereit sind, klicken Sie "Aufnahme" und singen Sie Ihr Lieblingslied.</t>
+  </si>
+  <si>
+    <t>Singen Sie das Lied!</t>
+  </si>
+  <si>
+    <t>Wenn Sie bereit sind, klicken Sie "Aufnahme und singen Sie das Lied nach.</t>
+  </si>
+  <si>
+    <t>Singen Sie Happy Birthday</t>
+  </si>
+  <si>
+    <t>Wenn Sie bereit sind, klicken Sie "Aufnahme" und singen Sie Happy Birthday.</t>
+  </si>
+  <si>
+    <t>lv</t>
+  </si>
+  <si>
+    <t>Dziedāšanas prasmju novērtējums</t>
+  </si>
+  <si>
+    <t>Esi sveicināts</t>
+  </si>
+  <si>
+    <t>Šajā testā tev vajadzēs atkārtot dažas skaņas un melodijas, kuras mēs tev nospēlēsim. Tas nekas, ja tev šķiet, ka tavas dziedāšanas prasmes nav labas. Pirmajā dziedāšanas testā daži piemēri, iespējams, tev liksies vieglāki un citi sarežģītāki. Šis tests pielāgojas tavam sniegumam, tādēļ katrā izmēģinājuma reizē kļūs arvien sarežģītāk. Mēģini parādīt vislabāko rezultātu.</t>
+  </si>
+  <si>
+    <t>Lūdzu, uzmanīgi izlasi instrukcijas.</t>
+  </si>
+  <si>
+    <t>Kā dziedāt</t>
+  </si>
+  <si>
+    <t>Tev būs jāatkārto dažas skaņas. Lūdzu, nodziedi šīs skaņas ar zilbi "ma"</t>
+  </si>
+  <si>
+    <t>Mēģini veidot skaņas stabili, bez vibrācijas. Tas nozīmē, lai skaņas "nedrebētu". Dators vislabāk spēj izanalizēt "taisnas" skaņas</t>
+  </si>
+  <si>
+    <t>Dziedi tieši mikrofonā, neatrodies pārāk tālu no tā. Attālums ap 30 cm ir atbilstošs.</t>
+  </si>
+  <si>
+    <t>Tev var būt</t>
+  </si>
+  <si>
+    <t>Tev būs</t>
+  </si>
+  <si>
+    <t>iet, lai iegūtu pēc iespējas labāku melodiju</t>
+  </si>
+  <si>
+    <t>ej, lai iegūtu pēc iespējas labāku melodiju</t>
+  </si>
+  <si>
+    <t>Tu vari izmēģināt tik daudz reižu, cik tev ir nepieciešams. Mums ir svarīgi redzēt tava sniegumu uzlabojumu katrā izmēģinājuma reizē.</t>
+  </si>
+  <si>
+    <t>Spēlē / atskaņo skaņu un dziedi līdzi</t>
+  </si>
+  <si>
+    <t>Dziedi melodiju, kuru tu dzirdi</t>
+  </si>
+  <si>
+    <t>Šajās izmēģinājumu reizēs tev jāspiež poga, lai dzirdētu melodiju.</t>
+  </si>
+  <si>
+    <t>Pēc tam, kad noklausīsies melodiju, mēģini to atkārtot, cik vien labi vari, tad nospied "Stop". Tu vari izmēģināt 3 reizes. Tas nekas, ja tev liekas, ka nesanāks, mēģini parādīt vislabāko sniegumu!</t>
+  </si>
+  <si>
+    <t>Dziedāšanas Prasmju Novērtējums</t>
+  </si>
+  <si>
+    <t>Ievadu lietotājvārdu, lai skatītu rezultātu tabulu</t>
+  </si>
+  <si>
+    <t>Dziedi savu mīļāko dziesmu!</t>
+  </si>
+  <si>
+    <t>Kad tu esi gatavs, spied "Ierakstīt" un dziedi savu mīļāko dziesmu.</t>
+  </si>
+  <si>
+    <t>Dziedi dziesmu!</t>
+  </si>
+  <si>
+    <t>Kad tu esi gatavs, spied "Ierakstīt" un dziedi dziesmu, kuru dzirdēji.</t>
+  </si>
+  <si>
+    <t>Dziedi "Happy Birthday"</t>
+  </si>
+  <si>
+    <t>Kad tu esi gatavs, spied "Ierakstīt" un dziedi "Happy Birthday", pēc tam, kad būsi to dzirdējis.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -297,8 +414,28 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,12 +456,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFBDC0BF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -494,13 +637,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA5A5A5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -555,27 +752,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1708,19 +1922,20 @@
   </sheetPr>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27.33203125" style="1" customWidth="1"/>
     <col min="2" max="4" width="166.6640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.33203125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="8.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1728,31 +1943,35 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="29" t="s">
+        <v>95</v>
+      </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1760,15 +1979,17 @@
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="D3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>97</v>
+      </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1778,13 +1999,15 @@
       <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="30" t="s">
+        <v>98</v>
+      </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1794,13 +2017,15 @@
       <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1810,13 +2035,15 @@
       <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="30" t="s">
+        <v>100</v>
+      </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
@@ -1826,302 +2053,354 @@
       <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="C9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="D9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="E9" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="D10" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="C11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="D11" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
+      <c r="C12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="D12" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+      <c r="C13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
+      <c r="C14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="D14" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="C15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="D15" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="E15" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
+      <c r="C16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="D16" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="E16" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+      <c r="C17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="D17" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="E17" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
+      <c r="C18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="D18" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="11"/>
+      <c r="D19" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>113</v>
+      </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="22" t="s">
+      <c r="B21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12" t="s">
+      <c r="C22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="C23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C24" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12" t="s">
+      <c r="D24" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="13" t="s">
+      <c r="B26" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C26" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="11"/>
+      <c r="D26" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>